<commit_message>
style: Fix spelling mistake in excel template #71
</commit_message>
<xml_diff>
--- a/Project/prototipo/src/main/resources/plantilla_excel.xlsx
+++ b/Project/prototipo/src/main/resources/plantilla_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\eLearningQA\Project\prototipo\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86150EA-89D4-4038-A7C7-65A3E377787B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA89C144-C5AE-4078-ADF0-9D550D52F49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1D2E916D-6742-41CB-A7BA-74AF9625EFBF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1D2E916D-6742-41CB-A7BA-74AF9625EFBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
     <t>Diseño</t>
   </si>
   <si>
-    <t>Se utilizan encuestas de opinió</t>
+    <t>Se utilizan encuestas de opinión</t>
   </si>
 </sst>
 </file>
@@ -318,18 +318,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -907,7 +896,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,6 +1077,16 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B4:B11 B13:B17 B19:B25 B27:B28">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF0000"/>
+        <color theme="9"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B13:B17">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -1098,16 +1097,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B11 B13:B17 B19:B25 B27:B28">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFFF0000"/>
-        <color theme="9"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>